<commit_message>
Update _New Splits Datasets for JRC2018.xlsx
</commit_message>
<xml_diff>
--- a/src/resources/_New Splits Datasets for JRC2018.xlsx
+++ b/src/resources/_New Splits Datasets for JRC2018.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexmclachlan/Documents/VFB/VFB_Curation/JRC2018 Splits/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adm71/Documents/GitHub/FlyLight-Split-GAL4-Curation/src/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{579D0317-4302-6A4E-8304-1DBC58255D83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{426F066D-D64D-4F49-A3DE-B64464EB2FE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29780" yWindow="11580" windowWidth="30400" windowHeight="9140" xr2:uid="{CF8C074D-91A3-E545-9320-0AF5836B951A}"/>
+    <workbookView xWindow="24680" yWindow="9360" windowWidth="20780" windowHeight="14760" xr2:uid="{CF8C074D-91A3-E545-9320-0AF5836B951A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="64">
   <si>
     <t>Missing ROIs</t>
   </si>
@@ -222,6 +222,9 @@
   </si>
   <si>
     <t>split GAL4 control, nothing found</t>
+  </si>
+  <si>
+    <t>Manual</t>
   </si>
 </sst>
 </file>
@@ -584,8 +587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A4C1771-3738-1C4C-9CC8-EAD945D9C251}">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -597,7 +600,7 @@
     <col min="5" max="5" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="32.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5" style="2" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="33.5" style="2" bestFit="1" customWidth="1"/>
@@ -994,7 +997,7 @@
         <v>6</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>6</v>
+        <v>63</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Split curation with slide codes update
</commit_message>
<xml_diff>
--- a/src/resources/_New Splits Datasets for JRC2018.xlsx
+++ b/src/resources/_New Splits Datasets for JRC2018.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adm71/Documents/GitHub/FlyLight-Split-GAL4-Curation/src/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76CA2088-DFED-A044-B637-89A9FC8C2D7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20916F18-2731-5043-A53C-D6D61837803F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17180" yWindow="12440" windowWidth="20780" windowHeight="14760" xr2:uid="{CF8C074D-91A3-E545-9320-0AF5836B951A}"/>
+    <workbookView xWindow="1060" yWindow="17240" windowWidth="20220" windowHeight="14760" xr2:uid="{CF8C074D-91A3-E545-9320-0AF5836B951A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="74">
   <si>
     <t>Missing ROIs</t>
   </si>
@@ -228,13 +228,34 @@
     <t>Manual</t>
   </si>
   <si>
-    <t>no Loaded</t>
-  </si>
-  <si>
-    <t>no New</t>
-  </si>
-  <si>
-    <t>Diff</t>
+    <t>Brain</t>
+  </si>
+  <si>
+    <t>VNC</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Second batch</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>old</t>
+  </si>
+  <si>
+    <t>LH2223/Lh732 hemi missing</t>
+  </si>
+  <si>
+    <t>No rows, not loaded</t>
+  </si>
+  <si>
+    <t>Loaded to Dolan2019</t>
+  </si>
+  <si>
+    <t>Passed test</t>
   </si>
 </sst>
 </file>
@@ -595,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A4C1771-3738-1C4C-9CC8-EAD945D9C251}">
-  <dimension ref="A1:P13"/>
+  <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -606,20 +627,26 @@
     <col min="1" max="1" width="26" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31" style="2" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="2" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" style="2" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="32.83203125" style="2" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="8.5" style="2" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="11.33203125" style="2" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="24" style="2" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="15.83203125" style="2" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="33.5" style="2" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="5.33203125" style="2" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="28.5" style="2" hidden="1" customWidth="1"/>
-    <col min="14" max="16384" width="10.83203125" style="2"/>
+    <col min="11" max="11" width="33.5" style="2" customWidth="1"/>
+    <col min="12" max="12" width="5.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.6640625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="5.33203125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="28.5" style="2" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="6.33203125" style="2" customWidth="1"/>
+    <col min="18" max="18" width="28.5" style="2" customWidth="1"/>
+    <col min="19" max="19" width="24.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>33</v>
       </c>
@@ -654,19 +681,25 @@
         <v>52</v>
       </c>
       <c r="L1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>66</v>
+      <c r="Q1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>28</v>
       </c>
@@ -700,11 +733,27 @@
       <c r="K2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>3</v>
+      <c r="L2" s="2">
+        <v>88</v>
+      </c>
+      <c r="M2" s="2">
+        <v>12</v>
+      </c>
+      <c r="N2" s="2">
+        <f>SUM(L2:M2)</f>
+        <v>100</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>188</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>27</v>
       </c>
@@ -735,11 +784,27 @@
       <c r="K3" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="L3" s="2" t="s">
-        <v>3</v>
+      <c r="L3" s="2">
+        <v>20</v>
+      </c>
+      <c r="M3" s="2">
+        <v>1</v>
+      </c>
+      <c r="N3" s="2">
+        <f t="shared" ref="N3:N12" si="0">SUM(L3:M3)</f>
+        <v>21</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>40</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>26</v>
       </c>
@@ -770,11 +835,27 @@
       <c r="K4" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="L4" s="2" t="s">
-        <v>3</v>
+      <c r="L4" s="2">
+        <v>32</v>
+      </c>
+      <c r="M4" s="2">
+        <v>31</v>
+      </c>
+      <c r="N4" s="2">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>0</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>25</v>
       </c>
@@ -805,11 +886,27 @@
       <c r="K5" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="L5" s="2" t="s">
-        <v>3</v>
+      <c r="L5" s="2">
+        <v>7</v>
+      </c>
+      <c r="M5" s="2">
+        <v>1</v>
+      </c>
+      <c r="N5" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>18</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>24</v>
       </c>
@@ -844,13 +941,28 @@
         <v>55</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>3</v>
+        <v>66</v>
       </c>
       <c r="M6" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="P6" s="2" t="s">
         <v>61</v>
       </c>
+      <c r="Q6" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>72</v>
+      </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -881,22 +993,27 @@
       <c r="K7" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="L7" s="2" t="s">
-        <v>3</v>
+      <c r="L7" s="2">
+        <v>629</v>
+      </c>
+      <c r="M7" s="2">
+        <v>326</v>
       </c>
       <c r="N7" s="2">
-        <f>326+629</f>
+        <f t="shared" si="0"/>
         <v>955</v>
       </c>
-      <c r="O7" s="2">
-        <v>1207</v>
-      </c>
-      <c r="P7" s="2">
-        <f>O7-N7</f>
-        <v>252</v>
+      <c r="O7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>838</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -930,14 +1047,30 @@
       <c r="K8" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="L8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="M8" s="2" t="s">
+      <c r="L8" s="2">
+        <v>2</v>
+      </c>
+      <c r="M8" s="2">
+        <v>0</v>
+      </c>
+      <c r="N8" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="P8" s="2" t="s">
         <v>62</v>
       </c>
+      <c r="Q8" s="2">
+        <v>4</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>73</v>
+      </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
@@ -968,11 +1101,27 @@
       <c r="K9" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="L9" s="2" t="s">
-        <v>3</v>
+      <c r="L9" s="2">
+        <v>3</v>
+      </c>
+      <c r="M9" s="2">
+        <v>1</v>
+      </c>
+      <c r="N9" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>8</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
@@ -1003,11 +1152,27 @@
       <c r="K10" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="L10" s="2" t="s">
-        <v>3</v>
+      <c r="L10" s="2">
+        <v>75</v>
+      </c>
+      <c r="M10" s="2">
+        <v>12</v>
+      </c>
+      <c r="N10" s="2">
+        <f t="shared" si="0"/>
+        <v>87</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>189</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
@@ -1041,11 +1206,27 @@
       <c r="K11" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="L11" s="2" t="s">
-        <v>3</v>
+      <c r="L11" s="2">
+        <v>282</v>
+      </c>
+      <c r="M11" s="2">
+        <v>82</v>
+      </c>
+      <c r="N11" s="2">
+        <f t="shared" si="0"/>
+        <v>364</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>497</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
@@ -1076,14 +1257,24 @@
       <c r="K12" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="L12" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="N13" s="2">
-        <f>1280+601</f>
-        <v>1881</v>
+      <c r="L12" s="2">
+        <v>125</v>
+      </c>
+      <c r="M12" s="2">
+        <v>122</v>
+      </c>
+      <c r="N12" s="2">
+        <f t="shared" si="0"/>
+        <v>247</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>256</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
script update and archiving
</commit_message>
<xml_diff>
--- a/src/resources/_New Splits Datasets for JRC2018.xlsx
+++ b/src/resources/_New Splits Datasets for JRC2018.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adm71/Documents/GitHub/FlyLight-Split-GAL4-Curation/src/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexmclachlan/Documents/GitHub/FlyLight-Split-GAL4-Curation/src/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20916F18-2731-5043-A53C-D6D61837803F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{171AEB14-0958-D54C-9443-B6FC55F605BC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="17240" windowWidth="20220" windowHeight="14760" xr2:uid="{CF8C074D-91A3-E545-9320-0AF5836B951A}"/>
+    <workbookView xWindow="29920" yWindow="-3900" windowWidth="20120" windowHeight="13600" xr2:uid="{CF8C074D-91A3-E545-9320-0AF5836B951A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="78">
   <si>
     <t>Missing ROIs</t>
   </si>
@@ -201,12 +201,6 @@
     <t>No, all curated</t>
   </si>
   <si>
-    <t>Do I need to both this and the release?</t>
-  </si>
-  <si>
-    <t>Do I need to both this and the preprint?</t>
-  </si>
-  <si>
     <t>Not in flybase yet</t>
   </si>
   <si>
@@ -246,16 +240,34 @@
     <t>old</t>
   </si>
   <si>
-    <t>LH2223/Lh732 hemi missing</t>
-  </si>
-  <si>
-    <t>No rows, not loaded</t>
-  </si>
-  <si>
-    <t>Loaded to Dolan2019</t>
-  </si>
-  <si>
-    <t>Passed test</t>
+    <t>Second batch mkii</t>
+  </si>
+  <si>
+    <t>20x and 63x only when left_dorsal, ventral, right_dorsal tiles present</t>
+  </si>
+  <si>
+    <t>Deleted</t>
+  </si>
+  <si>
+    <t>Merge with pub ver</t>
+  </si>
+  <si>
+    <t>Merge with pre ver</t>
+  </si>
+  <si>
+    <t>Merge</t>
+  </si>
+  <si>
+    <t>Merged with Dolan2019</t>
+  </si>
+  <si>
+    <t>Loaded</t>
+  </si>
+  <si>
+    <t>Dropped as empty</t>
+  </si>
+  <si>
+    <t>Count</t>
   </si>
 </sst>
 </file>
@@ -616,10 +628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A4C1771-3738-1C4C-9CC8-EAD945D9C251}">
-  <dimension ref="A1:R12"/>
+  <dimension ref="A1:T15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -646,7 +658,7 @@
     <col min="20" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>33</v>
       </c>
@@ -681,25 +693,31 @@
         <v>52</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="Q1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="S1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="R1" s="2" t="s">
-        <v>67</v>
+      <c r="T1" s="2" t="s">
+        <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>28</v>
       </c>
@@ -725,7 +743,7 @@
         <v>3</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>39</v>
@@ -750,10 +768,16 @@
         <v>188</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="T2" s="2">
+        <v>188</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>27</v>
       </c>
@@ -801,15 +825,21 @@
         <v>40</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="T3" s="2">
+        <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C4" s="2">
         <v>0</v>
@@ -852,10 +882,16 @@
         <v>0</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="T4" s="2">
+        <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>25</v>
       </c>
@@ -903,15 +939,21 @@
         <v>18</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="T5" s="2">
+        <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C6" s="2">
         <v>57</v>
@@ -938,31 +980,37 @@
         <v>39</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="T6" s="2">
+        <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -1010,10 +1058,16 @@
         <v>838</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="T7" s="2">
+        <v>840</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -1061,16 +1115,22 @@
         <v>3</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="Q8" s="2">
         <v>4</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="T8" s="2">
+        <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
@@ -1118,10 +1178,16 @@
         <v>8</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
+      </c>
+      <c r="S9" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="T9" s="2">
+        <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
@@ -1169,10 +1235,16 @@
         <v>189</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="T10" s="2">
+        <v>126</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
@@ -1192,7 +1264,7 @@
         <v>6</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>6</v>
@@ -1201,10 +1273,10 @@
         <v>51</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="L11" s="2">
         <v>282</v>
@@ -1225,8 +1297,14 @@
       <c r="R11" s="2" t="s">
         <v>70</v>
       </c>
+      <c r="S11" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="T11" s="2">
+        <v>329</v>
+      </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
@@ -1274,7 +1352,24 @@
         <v>256</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
+      </c>
+      <c r="S12" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="T12" s="2">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S13" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T15" s="2">
+        <f>SUM(T2:T12)</f>
+        <v>1799</v>
       </c>
     </row>
   </sheetData>

</xml_diff>